<commit_message>
Change Some Edit to MaskEdit.
</commit_message>
<xml_diff>
--- a/FillWeatherStat/1.xlsx
+++ b/FillWeatherStat/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\shanzhashu\FillWeatherStat\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC8C9B6-CEF8-4FB0-BEA9-A8FC0B256246}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D68D9F-3714-4F92-9F51-8329886F21AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="21720" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,15 +102,10 @@
     <t>记录编号：G-7231-H(T)23030150101</t>
   </si>
   <si>
-    <t xml:space="preserve">名称：干体炉/精密二通道标准铂电阻温度表
-生产厂家：中环天仪（天津）气象仪器有限公司/深圳市艾依康仪器仪表科技有限公司
-型号：RTC-158/ TM-3022T
-编号：660836-01013/3022T66
-证书编号：GQJ(C)WD2021-0604
-检定/校准日期：2022年9月9日
-有效期至：2023年9月8日
-不确定度/最大允许误差：±0.05℃
-</t>
+    <t>气温：20℃     湿度：90％RH    风速：1.0m/s</t>
+  </si>
+  <si>
+    <t>□合格                  ☑ 不合格</t>
   </si>
   <si>
     <t xml:space="preserve">使用单位：上栗东源国家气象观测站 
@@ -122,12 +117,18 @@
 自动站型号：DZZ5
 区站号：J7231
 </t>
-  </si>
-  <si>
-    <t>气温：20℃     湿度：90％RH    风速：1.0m/s</t>
-  </si>
-  <si>
-    <t>□合格                  ☑ 不合格</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称：干体炉/精密二通道标准铂电阻温度表
+生产厂家：中环天仪（天津）气象仪器有限公司/深圳市艾依康仪器仪表科技有限公司
+型号：RTC-158/ TM-3022T
+编号：660836-01013/3022T66
+证书编号：GQJ(C)WD2023-0652/GQJ(C)WD2023-0653
+检定/校准日期：2023年9月22日/2023年9月20日
+有效期至：2024年9月21日/2024年9月19日
+不确定度/最大允许误差：±0.05℃</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -135,8 +136,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="178" formatCode="0.000_ "/>
-    <numFmt numFmtId="179" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -397,61 +398,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -475,11 +449,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -487,7 +470,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -831,7 +832,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -846,98 +847,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
+      <c r="B4" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="42">
         <v>0.54861111111111105</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="42">
         <v>0.65972222222222221</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="43"/>
     </row>
     <row r="6" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="17" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-    </row>
-    <row r="7" spans="1:6" ht="222.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="40"/>
-      <c r="B7" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="31"/>
+    </row>
+    <row r="7" spans="1:6" ht="252.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="33"/>
+      <c r="B7" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
+      <c r="B8" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
@@ -960,166 +961,166 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="25">
+      <c r="A10" s="21">
         <v>-10</v>
       </c>
       <c r="B10" s="13">
         <v>-9.9920000000000009</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="15">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="18">
         <f>AVERAGE(B10:B12)+C10</f>
         <v>-9.9953333333333347</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="15">
         <v>-10.113</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="18">
         <f>E10-D10</f>
         <v>-0.11766666666666481</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="25"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="13">
         <v>-9.9890000000000008</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="27"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="25"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="13">
         <v>-9.9960000000000004</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="28"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="25">
+      <c r="A13" s="21">
         <v>0</v>
       </c>
       <c r="B13" s="12">
         <v>2.4E-2</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="22">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="18">
         <f>AVERAGE(B13:B15)+C13</f>
         <v>2.4999999999999998E-2</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="15">
         <v>-8.8999999999999996E-2</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="18">
         <f>E13-D13</f>
         <v>-0.11399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="25"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="12">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="27"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="25"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="12">
         <v>3.1E-2</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="28"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="25">
+      <c r="A16" s="21">
         <v>30</v>
       </c>
       <c r="B16" s="12">
         <v>30.102</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="22">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="18">
         <f>AVERAGE(B16:B18)+C16</f>
         <v>30.083333333333332</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="15">
         <v>29.983000000000001</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="18">
         <f>E16-D16</f>
         <v>-0.10033333333333161</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="25"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="12">
         <v>30.094999999999999</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="25"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="12">
         <v>30.091999999999999</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="28"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="20" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="41"/>
     </row>
     <row r="20" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="31"/>
+      <c r="C20" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="22"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41"/>
     </row>
     <row r="21" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20" t="s">
+      <c r="B21" s="31"/>
+      <c r="C21" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="22"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
@@ -1132,31 +1133,13 @@
       <c r="D22" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="37">
         <v>45000</v>
       </c>
-      <c r="F22" s="16"/>
+      <c r="F22" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A3:F3"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B8:F8"/>
@@ -1173,6 +1156,24 @@
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F16:F18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.47244094488188998" right="0.39370078740157499" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>

</xml_diff>

<commit_message>
Fix more Pages Problem.
</commit_message>
<xml_diff>
--- a/FillWeatherStat/1.xlsx
+++ b/FillWeatherStat/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\shanzhashu\FillWeatherStat\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D68D9F-3714-4F92-9F51-8329886F21AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02A477C-F9F2-43CA-90F8-33EC48333717}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="21720" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -374,9 +374,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -404,6 +401,48 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -411,21 +450,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -449,47 +473,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,13 +831,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.25" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.25" style="9" customWidth="1"/>
     <col min="2" max="2" width="17.75" customWidth="1"/>
     <col min="3" max="3" width="20.25" customWidth="1"/>
     <col min="4" max="4" width="18.75" customWidth="1"/>
@@ -847,101 +847,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="35" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="22">
         <v>0.54861111111111105</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="22">
         <v>0.65972222222222221</v>
       </c>
-      <c r="F5" s="43"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="31"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" ht="252.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="33"/>
-      <c r="B7" s="27" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="27" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="29"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -961,185 +961,204 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="21">
+      <c r="A10" s="24">
         <v>-10</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>-9.9920000000000009</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="28">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="25">
         <f>AVERAGE(B10:B12)+C10</f>
         <v>-9.9953333333333347</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="28">
         <v>-10.113</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="25">
         <f>E10-D10</f>
         <v>-0.11766666666666481</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="21"/>
-      <c r="B11" s="13">
+      <c r="A11" s="24"/>
+      <c r="B11" s="12">
         <v>-9.9890000000000008</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="19"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="21"/>
-      <c r="B12" s="13">
+      <c r="A12" s="24"/>
+      <c r="B12" s="12">
         <v>-9.9960000000000004</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="20"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="21">
+      <c r="A13" s="24">
         <v>0</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <v>2.4E-2</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="42">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="25">
         <f>AVERAGE(B13:B15)+C13</f>
         <v>2.4999999999999998E-2</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="28">
         <v>-8.8999999999999996E-2</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="25">
         <f>E13-D13</f>
         <v>-0.11399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="21"/>
-      <c r="B14" s="12">
+      <c r="A14" s="24"/>
+      <c r="B14" s="11">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="19"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="21"/>
-      <c r="B15" s="12">
+      <c r="A15" s="24"/>
+      <c r="B15" s="11">
         <v>3.1E-2</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="20"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="21">
+      <c r="A16" s="24">
         <v>30</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>30.102</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="42">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="25">
         <f>AVERAGE(B16:B18)+C16</f>
         <v>30.083333333333332</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="28">
         <v>29.983000000000001</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="25">
         <f>E16-D16</f>
         <v>-0.10033333333333161</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="21"/>
-      <c r="B17" s="12">
+      <c r="A17" s="24"/>
+      <c r="B17" s="11">
         <v>30.094999999999999</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="19"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="26"/>
     </row>
     <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="21"/>
-      <c r="B18" s="12">
+      <c r="A18" s="24"/>
+      <c r="B18" s="11">
         <v>30.091999999999999</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="20"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="27"/>
     </row>
     <row r="19" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="39" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="39" t="s">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="39" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="11" t="s">
+      <c r="B22" s="43"/>
+      <c r="C22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="37">
+      <c r="E22" s="14">
         <v>45000</v>
       </c>
-      <c r="F22" s="38"/>
+      <c r="F22" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B8:F8"/>
@@ -1156,24 +1175,6 @@
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="F16:F18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.47244094488188998" right="0.39370078740157499" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>

</xml_diff>